<commit_message>
Add measured and compensated uncertainty estimates to stage_uncertainty.xlsx
</commit_message>
<xml_diff>
--- a/calibration/stage_uncertainty.xlsx
+++ b/calibration/stage_uncertainty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_papers\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D7D04B-9D62-427B-A283-2946C5C87529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DB8240-2465-45BD-8141-F14D9F9611C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4956" yWindow="840" windowWidth="27516" windowHeight="19140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7296" yWindow="984" windowWidth="30048" windowHeight="19524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
   <si>
     <t>Z axis</t>
   </si>
@@ -111,12 +111,6 @@
     <t>Moment is +/- 50mm Z travel</t>
   </si>
   <si>
-    <t>Combined uncertainty</t>
-  </si>
-  <si>
-    <t>Max error +/-</t>
-  </si>
-  <si>
     <t>Source fixture</t>
   </si>
   <si>
@@ -133,6 +127,96 @@
   </si>
   <si>
     <t>Ouch!</t>
+  </si>
+  <si>
+    <t>Spec max +/-</t>
+  </si>
+  <si>
+    <t>Measured +/-</t>
+  </si>
+  <si>
+    <t>Y off-axis non-repeatability (um)</t>
+  </si>
+  <si>
+    <t>Measure by</t>
+  </si>
+  <si>
+    <t>Gauge blocks</t>
+  </si>
+  <si>
+    <t>Use square and test X move deviation at 30, 60, 90</t>
+  </si>
+  <si>
+    <t>Runout in Rz alignment test</t>
+  </si>
+  <si>
+    <t>Interpretation</t>
+  </si>
+  <si>
+    <t>Off axis lateral?</t>
+  </si>
+  <si>
+    <t>Off axis vertical?</t>
+  </si>
+  <si>
+    <t>Square</t>
+  </si>
+  <si>
+    <t>Off axis, but per axis or combined?</t>
+  </si>
+  <si>
+    <t>Indicator</t>
+  </si>
+  <si>
+    <t>Indicator over moment</t>
+  </si>
+  <si>
+    <t>Rz center vs stage body?</t>
+  </si>
+  <si>
+    <t>Change in Rz runout vs Z height</t>
+  </si>
+  <si>
+    <t>XY deviation with no Z moment</t>
+  </si>
+  <si>
+    <t>Off-axis RxRy? Includes non-square of Rz vs base?</t>
+  </si>
+  <si>
+    <t>Fixture ball deviation across positions</t>
+  </si>
+  <si>
+    <t>Rocking test vs. square</t>
+  </si>
+  <si>
+    <t>Variation of Y indication by refixturing (includes Y move away and back)</t>
+  </si>
+  <si>
+    <t>Ignore: doesn't matter</t>
+  </si>
+  <si>
+    <t>Total indicator reading / 2</t>
+  </si>
+  <si>
+    <t>Measurement from pole top will include moment effects</t>
+  </si>
+  <si>
+    <t>Spec uncertainty</t>
+  </si>
+  <si>
+    <t>meas u^2</t>
+  </si>
+  <si>
+    <t>Measured u</t>
+  </si>
+  <si>
+    <t>Comp +/-</t>
+  </si>
+  <si>
+    <t>comp u^2</t>
+  </si>
+  <si>
+    <t>Compensated</t>
   </si>
 </sst>
 </file>
@@ -148,7 +232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,8 +245,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -324,11 +414,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -336,9 +465,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -346,12 +472,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -360,49 +480,72 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -684,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,381 +839,688 @@
     <col min="3" max="3" width="9.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" customWidth="1"/>
     <col min="5" max="5" width="12.44140625" customWidth="1"/>
-    <col min="6" max="6" width="35.21875" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="35.33203125" customWidth="1"/>
+    <col min="11" max="11" width="45" customWidth="1"/>
+    <col min="12" max="12" width="62.5546875" customWidth="1"/>
+    <col min="13" max="14" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D1" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" t="s">
+      <c r="E1" s="26"/>
+      <c r="G1" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="F2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="19"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="20"/>
-      <c r="B4" s="21" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="17"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="30"/>
+      <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="17">
         <v>15</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <f>(C4*0.000001)^2</f>
         <v>2.2499999999999997E-10</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="21" t="s">
+      <c r="E4" s="17"/>
+      <c r="F4" s="17">
+        <v>65</v>
+      </c>
+      <c r="G4" s="7">
+        <f>(F4*0.000001)^2</f>
+        <v>4.224999999999999E-9</v>
+      </c>
+      <c r="H4" s="17">
+        <f>F4/4</f>
+        <v>16.25</v>
+      </c>
+      <c r="I4" s="7">
+        <f>(H4*0.000001)^2</f>
+        <v>2.6406249999999993E-10</v>
+      </c>
+      <c r="J4" s="18"/>
+      <c r="K4" s="17"/>
+      <c r="L4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="30"/>
+      <c r="B5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="17">
         <v>8</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <f t="shared" ref="D5:D13" si="0">(C5*0.000001)^2</f>
         <v>6.3999999999999999E-11</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="23"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="21" t="s">
+      <c r="E5" s="17"/>
+      <c r="F5" s="17">
+        <v>110</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" ref="G5:G6" si="1">(F5*0.000001)^2</f>
+        <v>1.2099999999999998E-8</v>
+      </c>
+      <c r="H5" s="17">
+        <f>F5/4</f>
+        <v>27.5</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" ref="I5:I6" si="2">(H5*0.000001)^2</f>
+        <v>7.5624999999999984E-10</v>
+      </c>
+      <c r="J5" s="18"/>
+      <c r="K5" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="30"/>
+      <c r="B6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="17">
         <v>8</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <f t="shared" si="0"/>
         <v>6.3999999999999999E-11</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="5" t="s">
+      <c r="E6" s="17"/>
+      <c r="F6" s="17">
+        <v>20</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="1"/>
+        <v>3.9999999999999991E-10</v>
+      </c>
+      <c r="H6" s="17">
+        <v>20</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="2"/>
+        <v>3.9999999999999991E-10</v>
+      </c>
+      <c r="J6" s="18"/>
+      <c r="K6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="31"/>
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>5</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="25"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D7" s="6"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="17"/>
+      <c r="L7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="19"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="17"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="33"/>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="17">
         <v>12</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D10" s="7"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="17"/>
+      <c r="L10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="33"/>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="17">
         <v>291</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <f>(C11*0.000001*0.05)^2</f>
         <v>2.117025E-10</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="23" t="s">
+      <c r="E11" s="17"/>
+      <c r="F11" s="17">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7">
+        <f>(F11*0.000001*0.05)^2</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <f>(H11*0.000001*0.05)^2</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="K11" s="17"/>
+      <c r="L11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="33"/>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="17">
         <v>24</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <f t="shared" si="0"/>
         <v>5.7600000000000008E-10</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="23"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="17"/>
+      <c r="F12" s="17">
+        <v>109</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" ref="G12:G13" si="3">(F12*0.000001)^2</f>
+        <v>1.1880999999999999E-8</v>
+      </c>
+      <c r="H12" s="17">
+        <f>F12/4</f>
+        <v>27.25</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" ref="I12:I13" si="4">(H12*0.000001)^2</f>
+        <v>7.4256249999999994E-10</v>
+      </c>
+      <c r="J12" s="18"/>
+      <c r="K12" s="17"/>
+      <c r="L12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="34"/>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>76</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <f t="shared" si="0"/>
         <v>5.7759999999999983E-9</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="25"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
+        <v>14</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" si="3"/>
+        <v>1.96E-10</v>
+      </c>
+      <c r="H13" s="3">
+        <f>F13*2</f>
+        <v>28</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="4"/>
+        <v>7.8399999999999998E-10</v>
+      </c>
+      <c r="J13" s="19"/>
+      <c r="K13" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="19"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="17"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="33"/>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="17">
         <v>145</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="F16" s="23"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D16" s="7"/>
+      <c r="F16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="17"/>
+      <c r="L16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="33"/>
-      <c r="B17" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="27">
+      <c r="B17" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="21">
         <v>2900</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7">
         <f>(C17*0.000001)^2</f>
         <v>8.4099999999999991E-6</v>
       </c>
-      <c r="F17" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F17" s="21"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="K17" s="17"/>
+      <c r="L17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="17">
         <v>75</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <f>(C18*0.000001)^2</f>
         <v>5.6249999999999991E-9</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="23"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E18" s="7"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="L18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="33"/>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="17">
         <v>127</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="23"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="34"/>
-      <c r="B20" s="5" t="s">
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="L19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="33"/>
+      <c r="B20" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="17">
+        <v>15</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="17"/>
+      <c r="L20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="34"/>
+      <c r="B21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C21" s="3">
         <v>291</v>
       </c>
-      <c r="D20" s="7">
-        <f>(C20*0.000001*0.05)^2</f>
+      <c r="D21" s="6">
+        <f>(C21*0.000001*0.05)^2</f>
         <v>2.117025E-10</v>
       </c>
-      <c r="E20" s="7">
-        <f>(C20*0.000001)^2</f>
+      <c r="E21" s="6">
+        <f>(C21*0.000001)^2</f>
         <v>8.4680999999999989E-8</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F21" s="3"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="26" t="s">
+      <c r="K21" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="L21" s="25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C23" s="13"/>
+      <c r="D23" s="14">
+        <f>(F23*0.000001)^2</f>
+        <v>1.6899999999999999E-10</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13">
         <v>13</v>
       </c>
-      <c r="D22" s="18">
-        <f t="shared" ref="D22" si="1">(C22*0.000001)^2</f>
-        <v>1.6899999999999999E-10</v>
-      </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="19"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="31"/>
-      <c r="B23" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="4">
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="17"/>
+      <c r="L23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="36"/>
+      <c r="B24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3">
+        <f>(F24*0.000001*0.2)^2</f>
+        <v>3.9999999999999991E-10</v>
+      </c>
+      <c r="E24" s="6">
+        <f>(F24*0.000001)^2</f>
+        <v>9.9999999999999986E-9</v>
+      </c>
+      <c r="F24" s="3">
         <f>13/0.13</f>
         <v>100</v>
       </c>
-      <c r="D23" s="4">
-        <f>(C23*0.000001*0.2)^2</f>
+      <c r="G24" s="6"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24" s="17"/>
+      <c r="L24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14">
+        <f>(F26*0.000001)^2</f>
         <v>3.9999999999999991E-10</v>
       </c>
-      <c r="E23" s="7">
-        <f>(C23*0.000001)^2</f>
-        <v>9.9999999999999986E-9</v>
-      </c>
-      <c r="F23" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="17">
+      <c r="E26" s="13"/>
+      <c r="F26" s="13">
+        <v>20</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="17"/>
+      <c r="L26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="37"/>
+      <c r="B27" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="7">
+        <f>(F27*0.000001)^2</f>
+        <v>8.9999999999999985E-8</v>
+      </c>
+      <c r="F27" s="17">
+        <v>300</v>
+      </c>
+      <c r="G27" s="7"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="17"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="36"/>
+      <c r="B28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="6">
+        <f>(F28*0.000001)^2</f>
+        <v>1.6899999999999999E-10</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="22">
         <v>13</v>
       </c>
-      <c r="D25" s="18">
-        <f t="shared" ref="D25:D27" si="2">(C25*0.000001)^2</f>
-        <v>1.6899999999999999E-10</v>
-      </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="19"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="30"/>
-      <c r="B26" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="22">
-        <v>300</v>
-      </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="8">
-        <f>(C26*0.000001)^2</f>
-        <v>8.9999999999999985E-8</v>
-      </c>
-      <c r="F26" s="23"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="31"/>
-      <c r="B27" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="28">
-        <v>13</v>
-      </c>
-      <c r="D27" s="7">
-        <f t="shared" si="2"/>
-        <v>1.6899999999999999E-10</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="25"/>
-    </row>
-    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D29" s="11">
-        <f>SQRT(SUM($D4:$D27))*1000000</f>
-        <v>116.87773526211053</v>
-      </c>
-      <c r="E29" s="12">
-        <f>SQRT(SUM($E4:$E27))*1000000</f>
+      <c r="G28" s="3"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="17"/>
+      <c r="L28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D30" s="8">
+        <f>SQRT(SUM($D4:$D28))*1000000</f>
+        <v>117.86180466970627</v>
+      </c>
+      <c r="E30" s="9">
+        <f>SQRT(SUM($E4:$E28))*1000000</f>
         <v>2931.6686374827559</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D30" s="13" t="s">
+      <c r="G30" s="38">
+        <f>SQRT(SUM(G4:G13)+SUM(D15:D28))*1000000</f>
+        <v>189.1473037079831</v>
+      </c>
+      <c r="I30" s="38">
+        <f>SQRT(SUM(I4:I13)+SUM(D15:D28))*1000000</f>
+        <v>99.607115709672058</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D31" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E31" s="11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D31" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="10"/>
+      <c r="G31" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D32" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="28"/>
+      <c r="G32" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="I32" s="40" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A26:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished uncertainty discussion, updates to stage_uncertainty.xlsx.  Added uncertainty to table1_concentric_vs_dipole.xlsx.  Started adding references.
</commit_message>
<xml_diff>
--- a/calibration/stage_uncertainty.xlsx
+++ b/calibration/stage_uncertainty.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_papers\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DB8240-2465-45BD-8141-F14D9F9611C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{515B22F6-6E64-4A96-9CD3-17F58F71E2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7296" yWindow="984" windowWidth="30048" windowHeight="19524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="26580" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
   <si>
     <t>Z axis</t>
   </si>
@@ -162,9 +163,6 @@
     <t>Square</t>
   </si>
   <si>
-    <t>Off axis, but per axis or combined?</t>
-  </si>
-  <si>
     <t>Indicator</t>
   </si>
   <si>
@@ -217,6 +215,12 @@
   </si>
   <si>
     <t>Compensated</t>
+  </si>
+  <si>
+    <t>Interpreting as XY vector error</t>
+  </si>
+  <si>
+    <t>in meas case is absorbed into straight and flat</t>
   </si>
 </sst>
 </file>
@@ -504,48 +508,48 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -830,7 +834,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -850,15 +854,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="26"/>
+      <c r="E1" s="29"/>
       <c r="G1" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
         <v>20</v>
@@ -887,20 +891,20 @@
         <v>18</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I2" s="24" t="s">
         <v>18</v>
       </c>
       <c r="K2" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="L2" s="23" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -917,7 +921,7 @@
       <c r="K3" s="17"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
@@ -951,7 +955,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="30"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="16" t="s">
         <v>3</v>
       </c>
@@ -967,7 +971,7 @@
         <v>110</v>
       </c>
       <c r="G5" s="7">
-        <f t="shared" ref="G5:G6" si="1">(F5*0.000001)^2</f>
+        <f>(F5*0.000001)^2</f>
         <v>1.2099999999999998E-8</v>
       </c>
       <c r="H5" s="17">
@@ -975,7 +979,7 @@
         <v>27.5</v>
       </c>
       <c r="I5" s="7">
-        <f t="shared" ref="I5:I6" si="2">(H5*0.000001)^2</f>
+        <f>(H5*0.000001)^2</f>
         <v>7.5624999999999984E-10</v>
       </c>
       <c r="J5" s="18"/>
@@ -983,11 +987,11 @@
         <v>39</v>
       </c>
       <c r="L5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="30"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="16" t="s">
         <v>4</v>
       </c>
@@ -1003,14 +1007,14 @@
         <v>20</v>
       </c>
       <c r="G6" s="7">
-        <f t="shared" si="1"/>
+        <f>(F6*0.000001)^2</f>
         <v>3.9999999999999991E-10</v>
       </c>
       <c r="H6" s="17">
         <v>20</v>
       </c>
       <c r="I6" s="7">
-        <f t="shared" si="2"/>
+        <f>(H6*0.000001)^2</f>
         <v>3.9999999999999991E-10</v>
       </c>
       <c r="J6" s="18"/>
@@ -1018,11 +1022,11 @@
         <v>40</v>
       </c>
       <c r="L6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="31"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1038,14 +1042,14 @@
       <c r="J7" s="19"/>
       <c r="K7" s="17"/>
       <c r="L7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="35" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -1062,7 +1066,7 @@
       <c r="K9" s="17"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="33"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="16" t="s">
         <v>8</v>
       </c>
@@ -1078,11 +1082,11 @@
       <c r="J10" s="18"/>
       <c r="K10" s="17"/>
       <c r="L10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="33"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="16" t="s">
         <v>9</v>
       </c>
@@ -1111,13 +1115,15 @@
       <c r="J11" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="17"/>
+      <c r="K11" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="L11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="33"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="16" t="s">
         <v>2</v>
       </c>
@@ -1133,7 +1139,7 @@
         <v>109</v>
       </c>
       <c r="G12" s="7">
-        <f t="shared" ref="G12:G13" si="3">(F12*0.000001)^2</f>
+        <f>(F12*0.000001)^2</f>
         <v>1.1880999999999999E-8</v>
       </c>
       <c r="H12" s="17">
@@ -1141,7 +1147,7 @@
         <v>27.25</v>
       </c>
       <c r="I12" s="7">
-        <f t="shared" ref="I12:I13" si="4">(H12*0.000001)^2</f>
+        <f>(H12*0.000001)^2</f>
         <v>7.4256249999999994E-10</v>
       </c>
       <c r="J12" s="18"/>
@@ -1151,7 +1157,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="34"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1167,7 +1173,7 @@
         <v>14</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="3"/>
+        <f>(F13*0.000001)^2</f>
         <v>1.96E-10</v>
       </c>
       <c r="H13" s="3">
@@ -1175,22 +1181,22 @@
         <v>28</v>
       </c>
       <c r="I13" s="6">
-        <f t="shared" si="4"/>
+        <f>(H13*0.000001)^2</f>
         <v>7.8399999999999998E-10</v>
       </c>
       <c r="J13" s="19"/>
       <c r="K13" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="L13" t="s">
         <v>42</v>
-      </c>
-      <c r="L13" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="35" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -1207,7 +1213,7 @@
       <c r="K15" s="17"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="33"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="16" t="s">
         <v>13</v>
       </c>
@@ -1220,11 +1226,11 @@
       <c r="J16" s="18"/>
       <c r="K16" s="17"/>
       <c r="L16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="33"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="16" t="s">
         <v>29</v>
       </c>
@@ -1249,7 +1255,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="33"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="16" t="s">
         <v>14</v>
       </c>
@@ -1267,14 +1273,14 @@
       <c r="I18" s="7"/>
       <c r="J18" s="18"/>
       <c r="K18" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L18" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="33"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="16" t="s">
         <v>15</v>
       </c>
@@ -1289,14 +1295,14 @@
       <c r="I19" s="7"/>
       <c r="J19" s="18"/>
       <c r="K19" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="33"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="16" t="s">
         <v>33</v>
       </c>
@@ -1316,7 +1322,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="34"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="4" t="s">
         <v>16</v>
       </c>
@@ -1339,14 +1345,14 @@
         <v>24</v>
       </c>
       <c r="K21" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L21" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="38" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="20" t="s">
@@ -1367,11 +1373,11 @@
       <c r="J23" s="15"/>
       <c r="K23" s="17"/>
       <c r="L23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="36"/>
+      <c r="A24" s="39"/>
       <c r="B24" s="4" t="s">
         <v>26</v>
       </c>
@@ -1396,11 +1402,11 @@
       </c>
       <c r="K24" s="17"/>
       <c r="L24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="38" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="20" t="s">
@@ -1421,11 +1427,11 @@
       <c r="J26" s="15"/>
       <c r="K26" s="17"/>
       <c r="L26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="37"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="16" t="s">
         <v>26</v>
       </c>
@@ -1445,7 +1451,7 @@
       <c r="K27" s="17"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="36"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="4" t="s">
         <v>7</v>
       </c>
@@ -1464,7 +1470,7 @@
       <c r="J28" s="19"/>
       <c r="K28" s="17"/>
       <c r="L28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1477,11 +1483,11 @@
         <f>SQRT(SUM($E4:$E28))*1000000</f>
         <v>2931.6686374827559</v>
       </c>
-      <c r="G30" s="38">
+      <c r="G30" s="26">
         <f>SQRT(SUM(G4:G13)+SUM(D15:D28))*1000000</f>
         <v>189.1473037079831</v>
       </c>
-      <c r="I30" s="38">
+      <c r="I30" s="26">
         <f>SQRT(SUM(I4:I13)+SUM(D15:D28))*1000000</f>
         <v>99.607115709672058</v>
       </c>
@@ -1493,23 +1499,23 @@
       <c r="E31" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G31" s="39" t="s">
+      <c r="G31" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="I31" s="39" t="s">
+      <c r="I31" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D32" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="E32" s="28"/>
-      <c r="G32" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="I32" s="40" t="s">
-        <v>60</v>
+      <c r="D32" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="31"/>
+      <c r="G32" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="I32" s="28" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>